<commit_message>
fee management module working need improvement
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sparked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E9AAC7-CE0B-4F96-95D8-EB21D6BFBD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5843B0-FE61-47A9-81C3-A9DFCD5DD9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{933A9181-AFB9-4F5B-A640-491969775087}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>desicription of the issue</t>
   </si>
@@ -211,11 +211,20 @@
     <t>Student financial log in a SIS. The admin would like to keep a track of student financial log. Where he can add the student expenditure and the related description.</t>
   </si>
   <si>
+    <t xml:space="preserve">Fee structure setup flow - guide the admin in setting up the fee structure. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can choose which class he is applying the fees to. </t>
+  </si>
+  <si>
+    <t>admin can see who the students are in the current selections.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Start fee collection process 
 1. In the first step admin would have to choose the fee types
 2. then fee structure
 3. Generate invoices
-4. Then assign them to the students
+4. Then assign them to the students (class)
 6. setup deadline 
 7. Set up reminders systems
 5. Send notifications or convey them to the students via messsages or emails
@@ -228,7 +237,28 @@
 1. The </t>
   </si>
   <si>
-    <t xml:space="preserve">Fee structure setup flow - guide the admin in setting up the fee structure. </t>
+    <t>Add a new Start new session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fee sessions -  should we create something like fee sessions? The admin can give name and title for each of the session. For each session how many students are remaining. Who are they is shown. How much outstanding amount etc is remaining. </t>
+  </si>
+  <si>
+    <t>Fee sessions management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let the create fee session button be on the fee management dashboard. Lets create the Manage fee sessions page. This will show the list of fee session. Clicking on a specific fee session will open the fee session details page. </t>
+  </si>
+  <si>
+    <t>Make all the screens to have justify center</t>
+  </si>
+  <si>
+    <t>Backend tables are going to break at some point due to their ad-hoc nature</t>
+  </si>
+  <si>
+    <t>Fee structure model and concept not strongly implemented in the fee mangement.
+1. Fee structure has information that to which class and acadmeic it belongs to but its functionality is not determined by the class and academic year. Its just for information sake
+2. A particular fee structure can be assigned to any academic year or class there is no restriction for that. 
+3. A Fee structure will have a list of fee types and their associated amounts. This will give the total amount and the reason for the origin of such amount. Giving the parents a clear breakdown</t>
   </si>
 </sst>
 </file>
@@ -641,11 +671,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F5521-7AAE-41FB-8030-08BADBEB25B8}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,92 +824,83 @@
     </row>
     <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="E6" t="s">
         <v>14</v>
-      </c>
-      <c r="N5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="H6" t="s">
         <v>30</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O7" t="s">
         <v>18</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P7" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
       </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
       <c r="H8" t="s">
         <v>27</v>
       </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
@@ -891,16 +912,16 @@
     </row>
     <row r="10" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
@@ -909,104 +930,187 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
       </c>
       <c r="H12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>49</v>
+    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
+      <c r="A14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>27</v>
       </c>
-      <c r="J14" t="s">
+    </row>
+    <row r="15" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:9" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{098FCDF5-B87E-48A5-9B71-381656B9F3AC}">
-      <formula1>$M$2:$M$6</formula1>
+      <formula1>$M$2:$M$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{412001C6-818A-4687-9E23-5577B6BE22BC}">
-      <formula1>$O$2:$O$6</formula1>
+      <formula1>$O$2:$O$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{01376043-8D04-4BDE-A6B6-7F54DCD99DA0}">
-      <formula1>$N$2:$N$5</formula1>
+      <formula1>$N$2:$N$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{F5E70491-03F9-40F0-914B-85358F877E53}">
       <formula1>$P:$P</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{944D45D6-8B7D-4779-8A9B-F4407E00D4C3}"/>
+    <hyperlink ref="A14" r:id="rId1" xr:uid="{944D45D6-8B7D-4779-8A9B-F4407E00D4C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ledger implementation complete, need testing and QA
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sparked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5843B0-FE61-47A9-81C3-A9DFCD5DD9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D1A4F6-AC21-4381-B6FF-A043889B393B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{933A9181-AFB9-4F5B-A640-491969775087}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
   <si>
     <t>desicription of the issue</t>
   </si>
@@ -260,12 +260,91 @@
 2. A particular fee structure can be assigned to any academic year or class there is no restriction for that. 
 3. A Fee structure will have a list of fee types and their associated amounts. This will give the total amount and the reason for the origin of such amount. Giving the parents a clear breakdown</t>
   </si>
+  <si>
+    <t>simplify the repo structure. Remove unwanted. Make it lean</t>
+  </si>
+  <si>
+    <t>Archive feature for the fee sessions</t>
+  </si>
+  <si>
+    <t>Onboarding of the school flow and feature</t>
+  </si>
+  <si>
+    <t>Need to connect the ledger updates with the notification systems</t>
+  </si>
+  <si>
+    <t>Backend server timeout issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1 </t>
+  </si>
+  <si>
+    <t>improve the UI. Make it vertical span like forms</t>
+  </si>
+  <si>
+    <t>Provide clear instructuions on the purpose of each element in the step</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>Create a new fee structure and check if it is shown in the step 2</t>
+  </si>
+  <si>
+    <t>Option to make the fee structures active/inactive/delete/archive etc (ponder)</t>
+  </si>
+  <si>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>Check this thoroughly</t>
+  </si>
+  <si>
+    <t>selecting a class from the drop down should automatically show the list of students, no need to click on the filter</t>
+  </si>
+  <si>
+    <t>Let the filter button be for the name</t>
+  </si>
+  <si>
+    <t>What can be other filters for greater convinience</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Functionality test of the user flow </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create Session.</t>
+    </r>
+  </si>
+  <si>
+    <t>total calculation is flawed</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>The number of rows inserted int the student fee structure assignment should be modified. The way it is implemented is wrong.  Now, if the fee structure has 4 fee types then the for each student 4 rows are inserted</t>
+  </si>
+  <si>
+    <t>Add tutorials for each of the feature</t>
+  </si>
+  <si>
+    <t>Editing the fee structure does not reflect the changes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,8 +360,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +379,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -334,6 +427,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -671,11 +767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F5521-7AAE-41FB-8030-08BADBEB25B8}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,19 +1189,132 @@
         <v>66</v>
       </c>
     </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" s="10" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{098FCDF5-B87E-48A5-9B71-381656B9F3AC}">
+  <mergeCells count="1">
+    <mergeCell ref="A33:XFD33"/>
+  </mergeCells>
+  <dataValidations disablePrompts="1" count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E32 E34:E1048576" xr:uid="{098FCDF5-B87E-48A5-9B71-381656B9F3AC}">
       <formula1>$M$2:$M$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{412001C6-818A-4687-9E23-5577B6BE22BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G32 G34:G1048576" xr:uid="{412001C6-818A-4687-9E23-5577B6BE22BC}">
       <formula1>$O$2:$O$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{01376043-8D04-4BDE-A6B6-7F54DCD99DA0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F32 F34:F1048576" xr:uid="{01376043-8D04-4BDE-A6B6-7F54DCD99DA0}">
       <formula1>$N$2:$N$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{F5E70491-03F9-40F0-914B-85358F877E53}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H34:H1048576 H1:H32" xr:uid="{F5E70491-03F9-40F0-914B-85358F877E53}">
       <formula1>$P:$P</formula1>
     </dataValidation>
   </dataValidations>
@@ -1113,6 +1322,7 @@
     <hyperlink ref="A14" r:id="rId1" xr:uid="{944D45D6-8B7D-4779-8A9B-F4407E00D4C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>